<commit_message>
Add latest test result
</commit_message>
<xml_diff>
--- a/Plate-Recognition/识别结果.xlsx
+++ b/Plate-Recognition/识别结果.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9144" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Related Cut" sheetId="1" r:id="rId1"/>
     <sheet name="DFS Cut" sheetId="3" r:id="rId2"/>
     <sheet name="Rlt&amp;DFS" sheetId="4" r:id="rId3"/>
+    <sheet name="Rlt&amp;DFS-Modify" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="563">
   <si>
     <t>京N84E28</t>
   </si>
@@ -1549,6 +1550,194 @@
   <si>
     <t>综合准确率</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浙A1XU17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赣A1L828</t>
+  </si>
+  <si>
+    <t>湘KMZ821</t>
+  </si>
+  <si>
+    <t>豫P060HK</t>
+  </si>
+  <si>
+    <t>粤L8U618</t>
+  </si>
+  <si>
+    <t>鄂KGW523</t>
+  </si>
+  <si>
+    <t>晋A50957</t>
+  </si>
+  <si>
+    <t>鲁AR9Y81</t>
+  </si>
+  <si>
+    <t>鲁B035CZ</t>
+  </si>
+  <si>
+    <t>浙B7V239</t>
+  </si>
+  <si>
+    <t>晋ACP777</t>
+  </si>
+  <si>
+    <t>皖AHK771</t>
+  </si>
+  <si>
+    <t>皖D36855</t>
+  </si>
+  <si>
+    <t>苏MKKD92</t>
+  </si>
+  <si>
+    <t>鄂MLY87M</t>
+  </si>
+  <si>
+    <t>苏WYY407</t>
+  </si>
+  <si>
+    <t>苏MRRD4D</t>
+  </si>
+  <si>
+    <t>苏C1E953</t>
+  </si>
+  <si>
+    <t>鄂JAY352</t>
+  </si>
+  <si>
+    <t>鄂K4878U</t>
+  </si>
+  <si>
+    <t>宁QG197R</t>
+  </si>
+  <si>
+    <t>川LAA071</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>沪MJD399</t>
+  </si>
+  <si>
+    <t>宁NA66D9</t>
+  </si>
+  <si>
+    <t>烫烫烫</t>
+  </si>
+  <si>
+    <t>川AK0A67</t>
+  </si>
+  <si>
+    <t>豫HQH356</t>
+  </si>
+  <si>
+    <t>鄂RDP938</t>
+  </si>
+  <si>
+    <t>鲁B9DN33</t>
+  </si>
+  <si>
+    <t>鄂N84E28</t>
+  </si>
+  <si>
+    <t>辽F365F9</t>
+  </si>
+  <si>
+    <t>陕1LAA07</t>
+  </si>
+  <si>
+    <t>沪A17726</t>
+  </si>
+  <si>
+    <t>宁MD7369</t>
+  </si>
+  <si>
+    <t>宁NC1791</t>
+  </si>
+  <si>
+    <t>鲁A3QJ36</t>
+  </si>
+  <si>
+    <t>晋A5FY92</t>
+  </si>
+  <si>
+    <t>湘A7KF06</t>
+  </si>
+  <si>
+    <t>鲁A8AX26</t>
+  </si>
+  <si>
+    <t>鲁B629CZ</t>
+  </si>
+  <si>
+    <t>浙B6852T</t>
+  </si>
+  <si>
+    <t>鲁B1BY79</t>
+  </si>
+  <si>
+    <t>浙BKF78T</t>
+  </si>
+  <si>
+    <t>皖A24094</t>
+  </si>
+  <si>
+    <t>川EH2600</t>
+  </si>
+  <si>
+    <t>川KF723A</t>
+  </si>
+  <si>
+    <t>皖KH9713</t>
+  </si>
+  <si>
+    <t>琼KW7521</t>
+  </si>
+  <si>
+    <t>晋MFZ066</t>
+  </si>
+  <si>
+    <t>鄂NW9151</t>
+  </si>
+  <si>
+    <t>川A07K36</t>
+  </si>
+  <si>
+    <t>新NA08F6</t>
+  </si>
+  <si>
+    <t>陕A3MG97</t>
+  </si>
+  <si>
+    <t>赣A8A527</t>
+  </si>
+  <si>
+    <t>陕A8AT15</t>
+  </si>
+  <si>
+    <t>蒙NC357Y</t>
+  </si>
+  <si>
+    <t>蒙A668LA</t>
+  </si>
+  <si>
+    <t>晋GLH989</t>
+  </si>
+  <si>
+    <t>蒙AJ0186</t>
+  </si>
+  <si>
+    <t>陕E9A219</t>
+  </si>
+  <si>
+    <t>赣QZT277</t>
+  </si>
+  <si>
+    <t>赣RA217F</t>
   </si>
 </sst>
 </file>
@@ -1910,7 +2099,7 @@
   <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8933,7 +9122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -9444,7 +9633,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>501</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>296</v>
@@ -13061,4 +13250,3515 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I174"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="C2" s="1">
+        <f>IF(A2=B2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <f>IF(LEFT(A2, 1) = LEFT(B2, 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <f>(IF(LEFT(RIGHT(A2, 1), 1) = LEFT(RIGHT(B2, 1), 1), 1, 0)+IF(LEFT(RIGHT(A2, 2), 1) = LEFT(RIGHT(B2, 2), 1), 1, 0)+IF(LEFT(RIGHT(A2, 3), 1) = LEFT(RIGHT(B2, 3), 1), 1, 0)+IF(LEFT(RIGHT(A2, 4), 1) = LEFT(RIGHT(B2, 4), 1), 1, 0)+IF(LEFT(RIGHT(A2, 5), 1) = LEFT(RIGHT(B2, 5), 1), 1, 0)+IF(LEFT(RIGHT(A2, 6), 1) = LEFT(RIGHT(B2, 6), 1), 1, 0))/6</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <f>AVERAGE(C:C)</f>
+        <v>0.57558139534883723</v>
+      </c>
+      <c r="G2" s="4">
+        <f>AVERAGE(D:D)</f>
+        <v>0.66279069767441856</v>
+      </c>
+      <c r="H2" s="4">
+        <f>AVERAGE(E:E)</f>
+        <v>0.93023255813953487</v>
+      </c>
+      <c r="I2" s="4">
+        <f>(G2+H2*6)/7</f>
+        <v>0.89202657807308972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C66" si="0">IF(A3=B3,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D66" si="1">IF(LEFT(A3, 1) = LEFT(B3, 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E66" si="2">(IF(LEFT(RIGHT(A3, 1), 1) = LEFT(RIGHT(B3, 1), 1), 1, 0)+IF(LEFT(RIGHT(A3, 2), 1) = LEFT(RIGHT(B3, 2), 1), 1, 0)+IF(LEFT(RIGHT(A3, 3), 1) = LEFT(RIGHT(B3, 3), 1), 1, 0)+IF(LEFT(RIGHT(A3, 4), 1) = LEFT(RIGHT(B3, 4), 1), 1, 0)+IF(LEFT(RIGHT(A3, 5), 1) = LEFT(RIGHT(B3, 5), 1), 1, 0)+IF(LEFT(RIGHT(A3, 6), 1) = LEFT(RIGHT(B3, 6), 1), 1, 0))/6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C58" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C59" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C61" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E62" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="C63" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E63" s="1">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E65" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="C66" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C67" s="1">
+        <f t="shared" ref="C67:C130" si="3">IF(A67=B67,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D130" si="4">IF(LEFT(A67, 1) = LEFT(B67, 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <f t="shared" ref="E67:E130" si="5">(IF(LEFT(RIGHT(A67, 1), 1) = LEFT(RIGHT(B67, 1), 1), 1, 0)+IF(LEFT(RIGHT(A67, 2), 1) = LEFT(RIGHT(B67, 2), 1), 1, 0)+IF(LEFT(RIGHT(A67, 3), 1) = LEFT(RIGHT(B67, 3), 1), 1, 0)+IF(LEFT(RIGHT(A67, 4), 1) = LEFT(RIGHT(B67, 4), 1), 1, 0)+IF(LEFT(RIGHT(A67, 5), 1) = LEFT(RIGHT(B67, 5), 1), 1, 0)+IF(LEFT(RIGHT(A67, 6), 1) = LEFT(RIGHT(B67, 6), 1), 1, 0))/6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="C68" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E68" s="1">
+        <f t="shared" si="5"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C69" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E70" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C71" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E71" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C72" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D72" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C73" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D73" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E73" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E74" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="C75" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E75" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C76" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E76" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C77" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E77" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C79" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C80" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D80" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E80" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E81" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C82" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D82" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E82" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C83" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E83" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C84" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D84" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E84" s="1">
+        <f t="shared" si="5"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E85" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C86" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E86" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C87" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D87" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E87" s="1">
+        <f t="shared" si="5"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E88" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C89" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D89" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E89" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C90" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D90" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E90" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="C91" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D91" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E91" s="1">
+        <f t="shared" si="5"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C92" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D92" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E92" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C93" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D93" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E93" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C94" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D94" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E94" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C95" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D95" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E95" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C96" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D96" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E96" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C97" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D97" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E97" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C98" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D98" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E98" s="1">
+        <f t="shared" si="5"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C99" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D99" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E99" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C100" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D100" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E100" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C101" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D101" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E101" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C102" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D102" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E102" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C103" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D103" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E103" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="C104" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D104" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E104" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="C105" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D105" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E105" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C106" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D106" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E106" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C107" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D107" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E107" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C108" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D108" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E108" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C109" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D109" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E109" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C110" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D110" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E110" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C111" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D111" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E111" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C112" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D112" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E112" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="C113" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D113" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E113" s="1">
+        <f t="shared" si="5"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C114" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D114" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E114" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C115" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D115" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E115" s="1">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="C116" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D116" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E116" s="1">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C117" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D117" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E117" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C118" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D118" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E118" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C119" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D119" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E119" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C120" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D120" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E120" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C121" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D121" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E121" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C122" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="D122" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E122" s="1">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C123" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D123" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E123" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C124" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D124" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E124" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C125" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D125" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E125" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C126" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D126" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E126" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C127" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D127" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E127" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C128" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D128" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E128" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C129" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D129" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E129" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C130" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D130" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E130" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C131" s="1">
+        <f t="shared" ref="C131:C170" si="6">IF(A131=B131,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D131" s="1">
+        <f t="shared" ref="D131:D170" si="7">IF(LEFT(A131, 1) = LEFT(B131, 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E131" s="1">
+        <f t="shared" ref="E131:E170" si="8">(IF(LEFT(RIGHT(A131, 1), 1) = LEFT(RIGHT(B131, 1), 1), 1, 0)+IF(LEFT(RIGHT(A131, 2), 1) = LEFT(RIGHT(B131, 2), 1), 1, 0)+IF(LEFT(RIGHT(A131, 3), 1) = LEFT(RIGHT(B131, 3), 1), 1, 0)+IF(LEFT(RIGHT(A131, 4), 1) = LEFT(RIGHT(B131, 4), 1), 1, 0)+IF(LEFT(RIGHT(A131, 5), 1) = LEFT(RIGHT(B131, 5), 1), 1, 0)+IF(LEFT(RIGHT(A131, 6), 1) = LEFT(RIGHT(B131, 6), 1), 1, 0))/6</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C132" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D132" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E132" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C133" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D133" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E133" s="1">
+        <f t="shared" si="8"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C134" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D134" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E134" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C135" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D135" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E135" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C136" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D136" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E136" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C137" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D137" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E137" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C138" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D138" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E138" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C139" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D139" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E139" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C140" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D140" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E140" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C141" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D141" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E141" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C142" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D142" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E142" s="1">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C143" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D143" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E143" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C144" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D144" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E144" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="C145" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D145" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E145" s="1">
+        <f t="shared" si="8"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C146" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D146" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E146" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C147" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D147" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E147" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C148" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D148" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E148" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C149" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D149" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E149" s="1">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C150" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D150" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E150" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C151" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D151" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E151" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="C152" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D152" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E152" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C153" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D153" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E153" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C154" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D154" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E154" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C155" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D155" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E155" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C156" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D156" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E156" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C157" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D157" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E157" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C158" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D158" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E158" s="1">
+        <f t="shared" si="8"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C159" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D159" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E159" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C160" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D160" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E160" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C161" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D161" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E161" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C162" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D162" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E162" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C163" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D163" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E163" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C164" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D164" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E164" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C165" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D165" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E165" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C166" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D166" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E166" s="1">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C167" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="D167" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E167" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C168" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D168" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E168" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C169" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D169" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E169" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C170" s="1">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D170" s="1">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="E170" s="1">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="C171" s="1">
+        <f t="shared" ref="C171:C173" si="9">IF(A171=B171,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D171" s="1">
+        <f t="shared" ref="D171:D173" si="10">IF(LEFT(A171, 1) = LEFT(B171, 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E171" s="1">
+        <f t="shared" ref="E171:E173" si="11">(IF(LEFT(RIGHT(A171, 1), 1) = LEFT(RIGHT(B171, 1), 1), 1, 0)+IF(LEFT(RIGHT(A171, 2), 1) = LEFT(RIGHT(B171, 2), 1), 1, 0)+IF(LEFT(RIGHT(A171, 3), 1) = LEFT(RIGHT(B171, 3), 1), 1, 0)+IF(LEFT(RIGHT(A171, 4), 1) = LEFT(RIGHT(B171, 4), 1), 1, 0)+IF(LEFT(RIGHT(A171, 5), 1) = LEFT(RIGHT(B171, 5), 1), 1, 0)+IF(LEFT(RIGHT(A171, 6), 1) = LEFT(RIGHT(B171, 6), 1), 1, 0))/6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C172" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D172" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E172" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C173" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D173" s="1">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="E173" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>